<commit_message>
Fix: Set scheduler timezone to UTC and add patient data
Co-authored-by: harshithame0517 <harshithame0517@gmail.com>
</commit_message>
<xml_diff>
--- a/data/calendar.xlsx
+++ b/data/calendar.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,36 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>b79f5a86</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>b2ea9becb2e0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Main Clinic</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-09-06T09:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>